<commit_message>
Aligned with possibly better partition and evaluated
</commit_message>
<xml_diff>
--- a/detailedComparison.xlsx
+++ b/detailedComparison.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab19451a4c9b763d/Documents/GitHub/knowledge-graph-partition-embedding/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Documents\GitHub\knowledge-graph-partition-embedding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{9C4A2F87-BAF3-444B-A3A3-A183E1A6401D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2932E9B-49A7-40E9-87C5-BBDAA6E98D2E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE310C95-BFDB-4948-99E4-F64D2914EE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F3AF854A-36B4-4775-B57F-8183FA708B74}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>Task</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Minedgecut_nd</t>
-  </si>
-  <si>
-    <t>Horizontal_Aligned0</t>
   </si>
   <si>
     <t>Minedgecut_aligned0</t>
@@ -154,14 +151,24 @@
   <si>
     <t>Sem</t>
   </si>
+  <si>
+    <t>Minedgecut_aligned3</t>
+  </si>
+  <si>
+    <t>Horizontal_aligned1</t>
+  </si>
+  <si>
+    <t>Horizontal_aligned0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00000000"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -227,8 +234,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -562,7 +569,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Horizontal_Aligned0</c:v>
+                  <c:v>Horizontal_aligned0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1227,7 +1234,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Horizontal_Aligned0</c:v>
+                  <c:v>Horizontal_aligned0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1881,7 +1888,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Horizontal_Aligned0</c:v>
+                  <c:v>Horizontal_aligned0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2502,7 +2509,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Horizontal_Aligned0</c:v>
+                  <c:v>Horizontal_aligned0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2546,7 +2553,7 @@
                 <c:pt idx="1">
                   <c:v>0.24717113431344501</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="2" formatCode="0.000000000">
                   <c:v>0.315991970009668</c:v>
                 </c:pt>
               </c:numCache>
@@ -2942,7 +2949,7 @@
                   <c:v>Minedgecut_nd</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Horizontal_Aligned0</c:v>
+                  <c:v>Horizontal_aligned0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Minedgecut_aligned0</c:v>
@@ -3443,7 +3450,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Horizontal_Aligned0</c:v>
+                  <c:v>Horizontal_aligned0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7637,10 +7644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CFF64A1-2666-40D3-B954-05F4271C476A}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7653,17 +7660,19 @@
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -7675,20 +7684,26 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
+      <c r="I1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="6" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2">
@@ -7706,13 +7721,18 @@
       <c r="H2">
         <v>0.68828571428571395</v>
       </c>
+      <c r="I2">
+        <v>0.68011904761904696</v>
+      </c>
+      <c r="J2">
+        <v>0.64328571428571402</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="6" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3">
@@ -7730,13 +7750,18 @@
       <c r="H3">
         <v>0.60320414587787996</v>
       </c>
+      <c r="I3">
+        <v>0.58665864813494895</v>
+      </c>
+      <c r="J3">
+        <v>0.59879692325968104</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="6" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D4">
@@ -7754,13 +7779,18 @@
       <c r="H4">
         <v>0.62274988692899103</v>
       </c>
+      <c r="I4">
+        <v>0.62077464788732395</v>
+      </c>
+      <c r="J4">
+        <v>0.62274988692899103</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="6" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D5">
@@ -7778,13 +7808,18 @@
       <c r="H5">
         <v>0.60947928331466905</v>
       </c>
+      <c r="I5">
+        <v>0.62384322508398604</v>
+      </c>
+      <c r="J5">
+        <v>0.61643784994400896</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="6" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D6">
@@ -7802,16 +7837,22 @@
       <c r="H6">
         <v>0.52610724156992805</v>
       </c>
+      <c r="I6">
+        <v>0.53210337202874503</v>
+      </c>
+      <c r="J6">
+        <v>0.53413764510779405</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>25</v>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="D7" s="1">
         <v>15.8807703684173</v>
@@ -7828,14 +7869,19 @@
       <c r="H7">
         <v>21.841848282905001</v>
       </c>
+      <c r="I7">
+        <v>20.882802893845898</v>
+      </c>
+      <c r="J7">
+        <v>21.3042208700167</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>25</v>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="D8">
         <v>20.162121369664501</v>
@@ -7852,14 +7898,19 @@
       <c r="H8">
         <v>23.237651414012799</v>
       </c>
+      <c r="I8">
+        <v>23.393744057163101</v>
+      </c>
+      <c r="J8">
+        <v>23.329553828015602</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>25</v>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="D9">
         <v>17.227857366831799</v>
@@ -7876,14 +7927,19 @@
       <c r="H9">
         <v>15.975267768039201</v>
       </c>
+      <c r="I9">
+        <v>15.6986692117743</v>
+      </c>
+      <c r="J9">
+        <v>15.743504914348501</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>25</v>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="D10">
         <v>64.370606495939697</v>
@@ -7900,14 +7956,19 @@
       <c r="H10">
         <v>75.211166028491505</v>
       </c>
+      <c r="I10">
+        <v>73.845443311231193</v>
+      </c>
+      <c r="J10">
+        <v>74.440390119815007</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>25</v>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="D11">
         <v>35.850490695925302</v>
@@ -7924,16 +7985,22 @@
       <c r="H11">
         <v>37.295294628137597</v>
       </c>
+      <c r="I11">
+        <v>38.902786564850203</v>
+      </c>
+      <c r="J11">
+        <v>38.684348160799502</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>26</v>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="D12">
         <v>0.77687354677159703</v>
@@ -7950,14 +8017,19 @@
       <c r="H12">
         <v>0.78402790198533401</v>
       </c>
+      <c r="I12" s="6">
+        <v>0.78268646038275702</v>
+      </c>
+      <c r="J12">
+        <v>0.78375961366481794</v>
+      </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>26</v>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="D13">
         <v>0.79304788213627997</v>
@@ -7974,14 +8046,19 @@
       <c r="H13">
         <v>0.53360957642725604</v>
       </c>
+      <c r="I13">
+        <v>0.53867403314917095</v>
+      </c>
+      <c r="J13">
+        <v>0.52647329650092101</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>26</v>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="D14">
         <v>0.81626553405694502</v>
@@ -7998,14 +8075,19 @@
       <c r="H14">
         <v>0.54727072518483599</v>
       </c>
+      <c r="I14">
+        <v>0.58879974830895099</v>
+      </c>
+      <c r="J14">
+        <v>0.56677678150070798</v>
+      </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>26</v>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="D15">
         <v>0.50499286733238202</v>
@@ -8022,16 +8104,22 @@
       <c r="H15">
         <v>0.527817403708987</v>
       </c>
+      <c r="I15">
+        <v>0.524013314312886</v>
+      </c>
+      <c r="J15">
+        <v>0.52757964812173097</v>
+      </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>27</v>
+      <c r="C16" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="D16">
         <v>0.45528207689882499</v>
@@ -8048,12 +8136,16 @@
       <c r="H16">
         <v>0.54314655211927099</v>
       </c>
+      <c r="I16">
+        <v>0.59282791926739298</v>
+      </c>
+      <c r="J16">
+        <v>0.552052157887441</v>
+      </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6" t="s">
-        <v>35</v>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="D17">
         <v>0.30403242508386602</v>
@@ -8070,12 +8162,16 @@
       <c r="H17">
         <v>0.38322716829930997</v>
       </c>
+      <c r="I17">
+        <v>0.414082373554651</v>
+      </c>
+      <c r="J17">
+        <v>0.36160967151851098</v>
+      </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6" t="s">
-        <v>28</v>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="D18">
         <v>0.35951458334449099</v>
@@ -8086,22 +8182,28 @@
       <c r="F18">
         <v>0.27374142849787603</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="6">
         <v>0.315991970009668</v>
       </c>
       <c r="H18">
         <v>0.44938346274795099</v>
       </c>
+      <c r="I18">
+        <v>0.48758979557494903</v>
+      </c>
+      <c r="J18">
+        <v>0.43698312231026898</v>
+      </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>29</v>
+      <c r="C19" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="D19">
         <v>0.51829573934837103</v>
@@ -8118,15 +8220,21 @@
       <c r="H19">
         <v>-0.40100250626566403</v>
       </c>
+      <c r="I19">
+        <v>-0.40100250626566403</v>
+      </c>
+      <c r="J19">
+        <v>-0.40100250626566403</v>
+      </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D20">
@@ -8144,13 +8252,18 @@
       <c r="H20">
         <v>0.62845849802371501</v>
       </c>
+      <c r="I20">
+        <v>0.57114624505928901</v>
+      </c>
+      <c r="J20">
+        <v>0.55533596837944699</v>
+      </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="6" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D21">
@@ -8168,13 +8281,18 @@
       <c r="H21">
         <v>0.34725906277630397</v>
       </c>
+      <c r="I21">
+        <v>0.37223695844385402</v>
+      </c>
+      <c r="J21">
+        <v>0.33333333333333298</v>
+      </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="6" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D22">
@@ -8192,13 +8310,18 @@
       <c r="H22">
         <v>1.3262599469495999E-2</v>
       </c>
+      <c r="I22">
+        <v>0.10212201591511801</v>
+      </c>
+      <c r="J22">
+        <v>0.110079575596817</v>
+      </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="6" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D23">
@@ -8215,6 +8338,12 @@
       </c>
       <c r="H23">
         <v>0.23162870648904199</v>
+      </c>
+      <c r="I23">
+        <v>0.19724967769660501</v>
+      </c>
+      <c r="J23">
+        <v>0.31070047271164603</v>
       </c>
     </row>
   </sheetData>
@@ -8310,7 +8439,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added results to detailed comparison
</commit_message>
<xml_diff>
--- a/detailedComparison.xlsx
+++ b/detailedComparison.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Documents\GitHub\knowledge-graph-partition-embedding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab19451a4c9b763d/Documents/GitHub/knowledge-graph-partition-embedding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE310C95-BFDB-4948-99E4-F64D2914EE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{8064D0E8-35CF-4CA8-9626-6C21C33DB4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F3AF854A-36B4-4775-B57F-8183FA708B74}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Classification_Diagram" sheetId="2" r:id="rId2"/>
-    <sheet name="Regression_Diagram" sheetId="3" r:id="rId3"/>
-    <sheet name="Clustering_Diagram" sheetId="4" r:id="rId4"/>
-    <sheet name="DocumentSimilarity_Diagram" sheetId="5" r:id="rId5"/>
-    <sheet name="EntitityRelatedness_Diagram" sheetId="6" r:id="rId6"/>
-    <sheet name="SemanticAnalogies_Diagram" sheetId="7" r:id="rId7"/>
+    <sheet name="Classification" sheetId="2" r:id="rId2"/>
+    <sheet name="Regression" sheetId="3" r:id="rId3"/>
+    <sheet name="Clustering" sheetId="4" r:id="rId4"/>
+    <sheet name="DocumentSimilarity" sheetId="5" r:id="rId5"/>
+    <sheet name="EntitityRelatedness" sheetId="6" r:id="rId6"/>
+    <sheet name="SemanticAnalogies" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
   <si>
     <t>Task</t>
   </si>
@@ -160,6 +160,24 @@
   <si>
     <t>Horizontal_aligned0</t>
   </si>
+  <si>
+    <t>Horizontal100_nd</t>
+  </si>
+  <si>
+    <t>Minedgecut100_nd</t>
+  </si>
+  <si>
+    <t>Horizontal100_aligned0</t>
+  </si>
+  <si>
+    <t>Horizontal100_aligned95</t>
+  </si>
+  <si>
+    <t>Minedgecut100_aligned0</t>
+  </si>
+  <si>
+    <t>Minedgecut100_aligned73</t>
+  </si>
 </sst>
 </file>
 
@@ -228,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -236,6 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -460,19 +479,19 @@
                 <c:formatCode>0.00000000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0.68719047619047602</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.58938880969351304</c:v>
+                  <c:v>0.66238095238095196</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59667438821572805</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>0.62077464788732395</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0.61054647256438899</c:v>
+                  <c:v>0.60969876819708801</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>0.53049891067538102</c:v>
+                  <c:v>0.54529408512990596</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -537,16 +556,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.68828571428571395</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.59362704918032705</c:v>
+                  <c:v>0.68538095238095198</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59896442147778495</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.62274988692899103</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.61822172452407598</c:v>
+                  <c:v>0.61454759238521794</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.53165616362631196</c:v>
@@ -711,6 +730,637 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-3F23-41DC-9012-E58904C57718}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal_aligned1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$2:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$I$2:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.68011904761904696</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.58665864813494895</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.62077464788732395</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.62384322508398604</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.53210337202874503</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4E1F-44D2-B83D-1FD5DD3002F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut_aligned3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$2:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$J$2:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.64328571428571402</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59879692325968104</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.62274988692899103</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61643784994400896</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.53413764510779405</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4E1F-44D2-B83D-1FD5DD3002F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal100_nd</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$2:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$K$2:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.60861904761904695</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59548794250415704</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.62448630136986305</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.590078387458006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52246766169154202</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4E1F-44D2-B83D-1FD5DD3002F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut100_nd</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$2:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$L$2:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.59054761904761899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.57556783083867902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.625342465753425</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58871108622620305</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.54288888888888798</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4E1F-44D2-B83D-1FD5DD3002F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal100_aligned0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$2:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$M$2:$M$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.62838095238095204</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59635513186029898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.62448630136986305</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.000000000">
+                  <c:v>0.585122060470324</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52795190713101103</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4E1F-44D2-B83D-1FD5DD3002F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut100_aligned0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$2:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$N$2:$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="0.000000000">
+                  <c:v>0.56952380952380899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59939296745070103</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.625342465753425</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.59398208286674103</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.53496296296296297</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-4E1F-44D2-B83D-1FD5DD3002F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal100_aligned95</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$2:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$O$2:$O$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.59145238095238095</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.605498930862437</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.62448630136986305</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.59408062709966303</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52951077943615199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-4E1F-44D2-B83D-1FD5DD3002F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut100_aligned73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$2:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$P$2:$P$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="0.000000000">
+                  <c:v>0.64749999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59732210738892799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.625342465753425</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.000000000">
+                  <c:v>0.57162486002239599</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52481481481481396</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-4E1F-44D2-B83D-1FD5DD3002F0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -782,7 +1432,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.8"/>
-          <c:min val="0.5"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1056,10 +1706,10 @@
                 <c:pt idx="2">
                   <c:v>17.227857366831799</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="3" formatCode="0.00000000">
                   <c:v>64.370606495939697</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="4" formatCode="0.00000000">
                   <c:v>35.850490695925302</c:v>
                 </c:pt>
               </c:numCache>
@@ -1125,19 +1775,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>18.970174483437699</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>23.7269711230526</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15.8483767552041</c:v>
+                  <c:v>18.351424380177502</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.710511878513</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.1197892860291</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76.628827004345197</c:v>
+                  <c:v>75.6303215715443</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.3214474796725</c:v>
+                  <c:v>39.916542192788</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1202,19 +1852,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>21.933145851503902</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>23.1040411120903</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15.9581835457551</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>74.596408874429898</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>37.072472390878303</c:v>
+                  <c:v>21.8603531353729</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.226037158334201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.807751049478499</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00000000">
+                  <c:v>74.410939602755704</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00000000">
+                  <c:v>37.263051200870002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1376,6 +2026,637 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-9161-4882-8DAC-F505CBC10BE6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal_aligned1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$7:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$I$7:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>20.882802893845898</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.393744057163101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.6986692117743</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>73.845443311231193</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.902786564850203</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3199-4844-A0FD-142138C78751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut_aligned3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$7:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$J$7:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>21.3042208700167</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.329553828015602</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.743504914348501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74.440390119815007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.684348160799502</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3199-4844-A0FD-142138C78751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal100_nd</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$7:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$K$7:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>19.644988651814199</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.721433231438098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.8325202779245</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83.381064910447705</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.675496506744103</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3199-4844-A0FD-142138C78751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut100_nd</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$7:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$L$7:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>22.7401986302784</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.016876190029599</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.1852298652062</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.4460998421808</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.686055216170701</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3199-4844-A0FD-142138C78751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal100_aligned0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$7:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$M$7:$M$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>20.329735431570001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.971208492907799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.026311443025701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>86.686386588869695</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.069290855976199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-3199-4844-A0FD-142138C78751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut100_aligned0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$7:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$N$7:$N$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>23.283493726035498</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.9443994730265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.227667746574099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82.023541661223703</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00000000">
+                  <c:v>39.434155497829998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-3199-4844-A0FD-142138C78751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal100_aligned95</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$7:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$O$7:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>23.206700205298201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.614087891271399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.9347164724387</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85.512644557264096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.189481806007599</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-3199-4844-A0FD-142138C78751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut100_aligned73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$7:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MetacriticMovies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MetacriticAlbums</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAUP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forbes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$P$7:$P$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>21.568127415810299</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.062302282357599</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.7497859937471</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85.099634984446695</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.603121260190797</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-3199-4844-A0FD-142138C78751}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1446,8 +2727,8 @@
         <c:axId val="368722992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="80"/>
-          <c:min val="10"/>
+          <c:max val="90"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1791,13 +3072,13 @@
                   <c:v>0.78554820246825297</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.51933701657458597</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.44502123643227898</c:v>
+                  <c:v>0.51657458563535896</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42881862513764402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.52448882548739895</c:v>
+                  <c:v>0.52520209224916703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1858,14 +3139,14 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.78608477910928298</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.51450276243093895</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.460751927009596</c:v>
+                <c:pt idx="0" formatCode="0.000000000">
+                  <c:v>0.78599534966911</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51473296500920795</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45162812647475198</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.52829291488349905</c:v>
@@ -2018,6 +3299,589 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-FF5C-4B36-9835-89CDBA69823B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal_aligned1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$12:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>citiesAndCountries</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cities2000AndCountries</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>citiesMoviesAlbumsCompaniesUnis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>teams</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$I$12:$I$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="0.000000000">
+                  <c:v>0.78268646038275702</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53867403314917095</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.58879974830895099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.524013314312886</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-803A-49B8-AE68-A06813D25EF2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut_aligned3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$12:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>citiesAndCountries</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cities2000AndCountries</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>citiesMoviesAlbumsCompaniesUnis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>teams</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$J$12:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.78375961366481794</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52647329650092101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56677678150070798</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52757964812173097</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-803A-49B8-AE68-A06813D25EF2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal100_nd</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$12:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>citiesAndCountries</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cities2000AndCountries</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>citiesMoviesAlbumsCompaniesUnis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>teams</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$K$12:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.78617420854945497</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51427255985266995</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>0.47805568664464398</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>0.525915359010937</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-803A-49B8-AE68-A06813D25EF2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut100_nd</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$12:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>citiesAndCountries</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cities2000AndCountries</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>citiesMoviesAlbumsCompaniesUnis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>teams</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$L$12:$L$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.78617420854945497</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51887661141804797</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45729117508258599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52377555872562997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-803A-49B8-AE68-A06813D25EF2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal100_aligned0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$12:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>citiesAndCountries</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cities2000AndCountries</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>citiesMoviesAlbumsCompaniesUnis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>teams</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$M$12:$M$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.78322303702378704</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53268876611418003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51706779927638702</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52543984783642395</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-803A-49B8-AE68-A06813D25EF2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut100_aligned0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$12:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>citiesAndCountries</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cities2000AndCountries</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>citiesMoviesAlbumsCompaniesUnis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>teams</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$N$12:$N$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="0.000000000">
+                  <c:v>0.78429619030584896</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51887661141804797</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53846153846153799</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52472658107465497</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-803A-49B8-AE68-A06813D25EF2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal100_aligned95</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$12:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>citiesAndCountries</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cities2000AndCountries</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>citiesMoviesAlbumsCompaniesUnis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>teams</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$O$12:$O$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.78358075478447498</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55616942909760503</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52713544124587097</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52543984783642395</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-803A-49B8-AE68-A06813D25EF2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut100_aligned73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$12:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>citiesAndCountries</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cities2000AndCountries</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>citiesMoviesAlbumsCompaniesUnis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>teams</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$P$12:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.78411733142550499</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53291896869244904</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51706779927638802</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52567760342367997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-803A-49B8-AE68-A06813D25EF2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2088,7 +3952,7 @@
         <c:axId val="368731632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.4"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2415,16 +4279,16 @@
             <c:numRef>
               <c:f>Data!$E$16:$E$18</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.42671107602158997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.31163060464238002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.36020242148222498</c:v>
+                  <c:v>0.42760951972364197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32858612958716898</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>0.371614296349565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2483,13 +4347,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.34310294776995298</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.22770807802653401</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.27374142849787603</c:v>
+                  <c:v>0.343668331822092</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21750598719014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26640534766639301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2627,6 +4491,541 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-9532-4E58-84B8-57A31FB22E86}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal_aligned1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$C$16:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Pearson correlation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Spearman correlation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Harmonic mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$I$16:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.59282791926739298</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.414082373554651</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.48758979557494903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EE87-4D91-875D-1CD63CC98D6A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut_aligned3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$C$16:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Pearson correlation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Spearman correlation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Harmonic mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$J$16:$J$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.552052157887441</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36160967151851098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43698312231026898</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EE87-4D91-875D-1CD63CC98D6A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal100_nd</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$C$16:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Pearson correlation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Spearman correlation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Harmonic mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$K$16:$K$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.31097776428604501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32608222692233801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.31835093492334599</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EE87-4D91-875D-1CD63CC98D6A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut100_nd</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$C$16:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Pearson correlation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Spearman correlation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Harmonic mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$L$16:$L$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.377036439334136</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32955534804950898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35170059208357202</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-EE87-4D91-875D-1CD63CC98D6A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal100_aligned0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$C$16:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Pearson correlation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Spearman correlation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Harmonic mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$M$16:$M$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.281177455745865</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27199647957356798</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.276510779757418</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-EE87-4D91-875D-1CD63CC98D6A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut100_aligned0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$C$16:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Pearson correlation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Spearman correlation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Harmonic mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$N$16:$N$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0" formatCode="0.000000000">
+                  <c:v>0.35120073951242098</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28369957772614102</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.313861873404435</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-EE87-4D91-875D-1CD63CC98D6A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal100_aligned95</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$C$16:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Pearson correlation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Spearman correlation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Harmonic mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$O$16:$O$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.36229243431055103</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.34394819350613998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.352882072749854</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-EE87-4D91-875D-1CD63CC98D6A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut100_aligned73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$C$16:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Pearson correlation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Spearman correlation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Harmonic mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$P$16:$P$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.386165924126325</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.387054367056131</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38660963517340302</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-EE87-4D91-875D-1CD63CC98D6A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2697,8 +5096,8 @@
         <c:axId val="418364672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.55000000000000004"/>
-          <c:min val="0.2"/>
+          <c:max val="0.60000000000000009"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2936,9 +5335,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$D$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
+              <c:f>Data!$D$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>Complete_nq</c:v>
                 </c:pt>
@@ -2953,30 +5352,78 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Minedgecut_aligned0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Horizontal_aligned1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Minedgecut_aligned3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Horizontal100_nd</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Minedgecut100_nd</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Horizontal100_aligned0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Minedgecut100_aligned0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Horizontal100_aligned95</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Minedgecut100_aligned73</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$D$19:$H$19</c:f>
+              <c:f>Data!$D$19:$P$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0.51829573934837103</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14887218045112699</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.22456140350877099</c:v>
+                  <c:v>0.13233082706766899</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000000000">
+                  <c:v>0.22406015037593899</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>-0.40100250626566403</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-0.40100250626566403</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.40100250626566403</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.40100250626566403</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.000000000">
+                  <c:v>-0.39999999999999902</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.42606516290726798</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.000000000">
+                  <c:v>-0.39999999999999902</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.40150375939849597</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.40050125313283202</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.40050125313283103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3350,16 +5797,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.55335968379446598</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.28404067197170602</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.3872679045093E-2</c:v>
+                  <c:v>0.57114624505928901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29310344827586199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9893899204244E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12720240653201501</c:v>
+                  <c:v>0.120326600773528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3421,16 +5868,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.48023715415019802</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.249115826702034</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.53557312252964395</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26105216622458</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000000000">
+                  <c:v>2.6525198938989998E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16931671680275001</c:v>
+                  <c:v>0.169746454662656</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3580,6 +6027,589 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-42E5-44B9-848F-C7DB57BFE706}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal_aligned1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$20:$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>all_capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>currency_entities</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>city_state_entities</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$I$20:$I$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.57114624505928901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.37223695844385402</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10212201591511801</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19724967769660501</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1CAB-4BC9-A274-369188EA500B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut_aligned3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$20:$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>all_capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>currency_entities</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>city_state_entities</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$J$20:$J$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.55533596837944699</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33333333333333298</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.110079575596817</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.31070047271164603</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1CAB-4BC9-A274-369188EA500B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal100_nd</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$20:$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>all_capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>currency_entities</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>city_state_entities</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$K$20:$K$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.5573122529644001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.10521662245799E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4588859416446E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9965620971208003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1CAB-4BC9-A274-369188EA500B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut100_nd</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$20:$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>all_capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>currency_entities</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>city_state_entities</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$L$20:$L$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.16403162055336001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4155614500441998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000000000">
+                  <c:v>3.9787798408489998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.4576708207992902E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1CAB-4BC9-A274-369188EA500B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal100_aligned0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$20:$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>all_capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>currency_entities</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>city_state_entities</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$M$20:$M$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.9525691699605001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.525198938992E-2</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000000000">
+                  <c:v>6.6312997347479996E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.254404813064E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-1CAB-4BC9-A274-369188EA500B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut100_aligned0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$20:$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>all_capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>currency_entities</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>city_state_entities</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$N$20:$N$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.158102766798419</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3050397877983997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000000000">
+                  <c:v>5.3050397877979997E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.5320154705630004E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-1CAB-4BC9-A274-369188EA500B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horizontal100_aligned95</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$20:$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>all_capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>currency_entities</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>city_state_entities</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$O$20:$O$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="0.000000000">
+                  <c:v>0.16798418972331999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8682581786029999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000000000">
+                  <c:v>6.6312997347479996E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.2625698324022006E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-1CAB-4BC9-A274-369188EA500B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minedgecut100_aligned73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$B$20:$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>all_capital_country_entities</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>currency_entities</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>city_state_entities</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$P$20:$P$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.122529644268775</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2272325375774E-2</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000000000">
+                  <c:v>3.9787798408489998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5006446067898999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-1CAB-4BC9-A274-369188EA500B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7644,27 +10674,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CFF64A1-2666-40D3-B954-05F4271C476A}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
     <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" customWidth="1"/>
+    <col min="16" max="16" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -7695,8 +10731,26 @@
       <c r="J1" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="K1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -7710,10 +10764,10 @@
         <v>0.79142857142857104</v>
       </c>
       <c r="E2">
-        <v>0.68719047619047602</v>
+        <v>0.66238095238095196</v>
       </c>
       <c r="F2">
-        <v>0.68828571428571395</v>
+        <v>0.68538095238095198</v>
       </c>
       <c r="G2">
         <v>0.68580952380952298</v>
@@ -7727,8 +10781,26 @@
       <c r="J2">
         <v>0.64328571428571402</v>
       </c>
+      <c r="K2">
+        <v>0.60861904761904695</v>
+      </c>
+      <c r="L2">
+        <v>0.59054761904761899</v>
+      </c>
+      <c r="M2">
+        <v>0.62838095238095204</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0.56952380952380899</v>
+      </c>
+      <c r="O2">
+        <v>0.59145238095238095</v>
+      </c>
+      <c r="P2" s="6">
+        <v>0.64749999999999996</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -7739,10 +10811,10 @@
         <v>0.71704561653599397</v>
       </c>
       <c r="E3" s="2">
-        <v>0.58938880969351304</v>
+        <v>0.59667438821572805</v>
       </c>
       <c r="F3">
-        <v>0.59362704918032705</v>
+        <v>0.59896442147778495</v>
       </c>
       <c r="G3">
         <v>0.58345034449988098</v>
@@ -7756,8 +10828,26 @@
       <c r="J3">
         <v>0.59879692325968104</v>
       </c>
+      <c r="K3">
+        <v>0.59548794250415704</v>
+      </c>
+      <c r="L3">
+        <v>0.57556783083867902</v>
+      </c>
+      <c r="M3">
+        <v>0.59635513186029898</v>
+      </c>
+      <c r="N3">
+        <v>0.59939296745070103</v>
+      </c>
+      <c r="O3">
+        <v>0.605498930862437</v>
+      </c>
+      <c r="P3">
+        <v>0.59732210738892799</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -7785,8 +10875,26 @@
       <c r="J4">
         <v>0.62274988692899103</v>
       </c>
+      <c r="K4">
+        <v>0.62448630136986305</v>
+      </c>
+      <c r="L4">
+        <v>0.625342465753425</v>
+      </c>
+      <c r="M4">
+        <v>0.62448630136986305</v>
+      </c>
+      <c r="N4">
+        <v>0.625342465753425</v>
+      </c>
+      <c r="O4">
+        <v>0.62448630136986305</v>
+      </c>
+      <c r="P4">
+        <v>0.625342465753425</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -7797,10 +10905,10 @@
         <v>0.67368794326241099</v>
       </c>
       <c r="E5">
-        <v>0.61054647256438899</v>
+        <v>0.60969876819708801</v>
       </c>
       <c r="F5">
-        <v>0.61822172452407598</v>
+        <v>0.61454759238521794</v>
       </c>
       <c r="G5">
         <v>0.61002015677491594</v>
@@ -7814,8 +10922,26 @@
       <c r="J5">
         <v>0.61643784994400896</v>
       </c>
+      <c r="K5">
+        <v>0.590078387458006</v>
+      </c>
+      <c r="L5">
+        <v>0.58871108622620305</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0.585122060470324</v>
+      </c>
+      <c r="N5">
+        <v>0.59398208286674103</v>
+      </c>
+      <c r="O5">
+        <v>0.59408062709966303</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0.57162486002239599</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -7826,7 +10952,7 @@
         <v>0.59360455702058701</v>
       </c>
       <c r="E6">
-        <v>0.53049891067538102</v>
+        <v>0.54529408512990596</v>
       </c>
       <c r="F6">
         <v>0.53165616362631196</v>
@@ -7843,8 +10969,26 @@
       <c r="J6">
         <v>0.53413764510779405</v>
       </c>
+      <c r="K6">
+        <v>0.52246766169154202</v>
+      </c>
+      <c r="L6">
+        <v>0.54288888888888798</v>
+      </c>
+      <c r="M6">
+        <v>0.52795190713101103</v>
+      </c>
+      <c r="N6">
+        <v>0.53496296296296297</v>
+      </c>
+      <c r="O6">
+        <v>0.52951077943615199</v>
+      </c>
+      <c r="P6">
+        <v>0.52481481481481396</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -7858,10 +11002,10 @@
         <v>15.8807703684173</v>
       </c>
       <c r="E7">
-        <v>18.970174483437699</v>
+        <v>18.351424380177502</v>
       </c>
       <c r="F7">
-        <v>21.933145851503902</v>
+        <v>21.8603531353729</v>
       </c>
       <c r="G7">
         <v>18.951428208305799</v>
@@ -7875,8 +11019,26 @@
       <c r="J7">
         <v>21.3042208700167</v>
       </c>
+      <c r="K7">
+        <v>19.644988651814199</v>
+      </c>
+      <c r="L7">
+        <v>22.7401986302784</v>
+      </c>
+      <c r="M7">
+        <v>20.329735431570001</v>
+      </c>
+      <c r="N7">
+        <v>23.283493726035498</v>
+      </c>
+      <c r="O7">
+        <v>23.206700205298201</v>
+      </c>
+      <c r="P7">
+        <v>21.568127415810299</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -7887,10 +11049,10 @@
         <v>20.162121369664501</v>
       </c>
       <c r="E8">
-        <v>23.7269711230526</v>
+        <v>23.710511878513</v>
       </c>
       <c r="F8">
-        <v>23.1040411120903</v>
+        <v>23.226037158334201</v>
       </c>
       <c r="G8">
         <v>23.341326493099402</v>
@@ -7904,8 +11066,26 @@
       <c r="J8">
         <v>23.329553828015602</v>
       </c>
+      <c r="K8">
+        <v>23.721433231438098</v>
+      </c>
+      <c r="L8">
+        <v>24.016876190029599</v>
+      </c>
+      <c r="M8">
+        <v>23.971208492907799</v>
+      </c>
+      <c r="N8">
+        <v>23.9443994730265</v>
+      </c>
+      <c r="O8">
+        <v>23.614087891271399</v>
+      </c>
+      <c r="P8">
+        <v>24.062302282357599</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -7916,10 +11096,10 @@
         <v>17.227857366831799</v>
       </c>
       <c r="E9">
-        <v>15.8483767552041</v>
+        <v>16.1197892860291</v>
       </c>
       <c r="F9">
-        <v>15.9581835457551</v>
+        <v>15.807751049478499</v>
       </c>
       <c r="G9">
         <v>16.212149818642899</v>
@@ -7933,22 +11113,40 @@
       <c r="J9">
         <v>15.743504914348501</v>
       </c>
+      <c r="K9">
+        <v>15.8325202779245</v>
+      </c>
+      <c r="L9">
+        <v>16.1852298652062</v>
+      </c>
+      <c r="M9">
+        <v>16.026311443025701</v>
+      </c>
+      <c r="N9">
+        <v>16.227667746574099</v>
+      </c>
+      <c r="O9">
+        <v>15.9347164724387</v>
+      </c>
+      <c r="P9">
+        <v>15.7497859937471</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>64.370606495939697</v>
       </c>
       <c r="E10">
-        <v>76.628827004345197</v>
-      </c>
-      <c r="F10">
-        <v>74.596408874429898</v>
+        <v>75.6303215715443</v>
+      </c>
+      <c r="F10" s="2">
+        <v>74.410939602755704</v>
       </c>
       <c r="G10">
         <v>77.053799090344398</v>
@@ -7962,22 +11160,40 @@
       <c r="J10">
         <v>74.440390119815007</v>
       </c>
+      <c r="K10">
+        <v>83.381064910447705</v>
+      </c>
+      <c r="L10">
+        <v>84.4460998421808</v>
+      </c>
+      <c r="M10">
+        <v>86.686386588869695</v>
+      </c>
+      <c r="N10">
+        <v>82.023541661223703</v>
+      </c>
+      <c r="O10">
+        <v>85.512644557264096</v>
+      </c>
+      <c r="P10">
+        <v>85.099634984446695</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>35.850490695925302</v>
       </c>
       <c r="E11">
-        <v>39.3214474796725</v>
-      </c>
-      <c r="F11">
-        <v>37.072472390878303</v>
+        <v>39.916542192788</v>
+      </c>
+      <c r="F11" s="2">
+        <v>37.263051200870002</v>
       </c>
       <c r="G11">
         <v>39.532124885228797</v>
@@ -7991,8 +11207,26 @@
       <c r="J11">
         <v>38.684348160799502</v>
       </c>
+      <c r="K11">
+        <v>39.675496506744103</v>
+      </c>
+      <c r="L11">
+        <v>39.686055216170701</v>
+      </c>
+      <c r="M11">
+        <v>39.069290855976199</v>
+      </c>
+      <c r="N11" s="2">
+        <v>39.434155497829998</v>
+      </c>
+      <c r="O11">
+        <v>39.189481806007599</v>
+      </c>
+      <c r="P11">
+        <v>39.603121260190797</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -8008,8 +11242,8 @@
       <c r="E12">
         <v>0.78554820246825297</v>
       </c>
-      <c r="F12">
-        <v>0.78608477910928298</v>
+      <c r="F12" s="6">
+        <v>0.78599534966911</v>
       </c>
       <c r="G12">
         <v>0.78349132534430299</v>
@@ -8023,8 +11257,26 @@
       <c r="J12">
         <v>0.78375961366481794</v>
       </c>
+      <c r="K12">
+        <v>0.78617420854945497</v>
+      </c>
+      <c r="L12">
+        <v>0.78617420854945497</v>
+      </c>
+      <c r="M12">
+        <v>0.78322303702378704</v>
+      </c>
+      <c r="N12" s="6">
+        <v>0.78429619030584896</v>
+      </c>
+      <c r="O12">
+        <v>0.78358075478447498</v>
+      </c>
+      <c r="P12">
+        <v>0.78411733142550499</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -8035,10 +11287,10 @@
         <v>0.79304788213627997</v>
       </c>
       <c r="E13">
-        <v>0.51933701657458597</v>
+        <v>0.51657458563535896</v>
       </c>
       <c r="F13">
-        <v>0.51450276243093895</v>
+        <v>0.51473296500920795</v>
       </c>
       <c r="G13">
         <v>0.51151012891344305</v>
@@ -8052,8 +11304,26 @@
       <c r="J13">
         <v>0.52647329650092101</v>
       </c>
+      <c r="K13" s="6">
+        <v>0.51427255985266995</v>
+      </c>
+      <c r="L13">
+        <v>0.51887661141804797</v>
+      </c>
+      <c r="M13">
+        <v>0.53268876611418003</v>
+      </c>
+      <c r="N13">
+        <v>0.51887661141804797</v>
+      </c>
+      <c r="O13">
+        <v>0.55616942909760503</v>
+      </c>
+      <c r="P13">
+        <v>0.53291896869244904</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>15</v>
       </c>
@@ -8064,10 +11334,10 @@
         <v>0.81626553405694502</v>
       </c>
       <c r="E14">
-        <v>0.44502123643227898</v>
+        <v>0.42881862513764402</v>
       </c>
       <c r="F14">
-        <v>0.460751927009596</v>
+        <v>0.45162812647475198</v>
       </c>
       <c r="G14">
         <v>0.55655183262545205</v>
@@ -8081,8 +11351,26 @@
       <c r="J14">
         <v>0.56677678150070798</v>
       </c>
+      <c r="K14">
+        <v>0.47805568664464398</v>
+      </c>
+      <c r="L14">
+        <v>0.45729117508258599</v>
+      </c>
+      <c r="M14">
+        <v>0.51706779927638702</v>
+      </c>
+      <c r="N14">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="O14">
+        <v>0.52713544124587097</v>
+      </c>
+      <c r="P14">
+        <v>0.51706779927638802</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>18</v>
       </c>
@@ -8093,7 +11381,7 @@
         <v>0.50499286733238202</v>
       </c>
       <c r="E15">
-        <v>0.52448882548739895</v>
+        <v>0.52520209224916703</v>
       </c>
       <c r="F15">
         <v>0.52829291488349905</v>
@@ -8110,8 +11398,26 @@
       <c r="J15">
         <v>0.52757964812173097</v>
       </c>
+      <c r="K15">
+        <v>0.525915359010937</v>
+      </c>
+      <c r="L15">
+        <v>0.52377555872562997</v>
+      </c>
+      <c r="M15">
+        <v>0.52543984783642395</v>
+      </c>
+      <c r="N15">
+        <v>0.52472658107465497</v>
+      </c>
+      <c r="O15">
+        <v>0.52543984783642395</v>
+      </c>
+      <c r="P15">
+        <v>0.52567760342367997</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -8124,11 +11430,11 @@
       <c r="D16">
         <v>0.45528207689882499</v>
       </c>
-      <c r="E16">
-        <v>0.42671107602158997</v>
+      <c r="E16" s="6">
+        <v>0.42760951972364197</v>
       </c>
       <c r="F16">
-        <v>0.34310294776995298</v>
+        <v>0.343668331822092</v>
       </c>
       <c r="G16">
         <v>0.43792521945173701</v>
@@ -8142,19 +11448,37 @@
       <c r="J16">
         <v>0.552052157887441</v>
       </c>
+      <c r="K16">
+        <v>0.31097776428604501</v>
+      </c>
+      <c r="L16">
+        <v>0.377036439334136</v>
+      </c>
+      <c r="M16">
+        <v>0.281177455745865</v>
+      </c>
+      <c r="N16" s="6">
+        <v>0.35120073951242098</v>
+      </c>
+      <c r="O16">
+        <v>0.36229243431055103</v>
+      </c>
+      <c r="P16">
+        <v>0.386165924126325</v>
+      </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C17" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D17">
         <v>0.30403242508386602</v>
       </c>
-      <c r="E17">
-        <v>0.31163060464238002</v>
+      <c r="E17" s="6">
+        <v>0.32858612958716898</v>
       </c>
       <c r="F17">
-        <v>0.22770807802653401</v>
+        <v>0.21750598719014</v>
       </c>
       <c r="G17">
         <v>0.24717113431344501</v>
@@ -8168,8 +11492,26 @@
       <c r="J17">
         <v>0.36160967151851098</v>
       </c>
+      <c r="K17">
+        <v>0.32608222692233801</v>
+      </c>
+      <c r="L17">
+        <v>0.32955534804950898</v>
+      </c>
+      <c r="M17" s="6">
+        <v>0.27199647957356798</v>
+      </c>
+      <c r="N17">
+        <v>0.28369957772614102</v>
+      </c>
+      <c r="O17">
+        <v>0.34394819350613998</v>
+      </c>
+      <c r="P17">
+        <v>0.387054367056131</v>
+      </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C18" s="5" t="s">
         <v>27</v>
       </c>
@@ -8177,10 +11519,10 @@
         <v>0.35951458334449099</v>
       </c>
       <c r="E18">
-        <v>0.36020242148222498</v>
+        <v>0.371614296349565</v>
       </c>
       <c r="F18">
-        <v>0.27374142849787603</v>
+        <v>0.26640534766639301</v>
       </c>
       <c r="G18" s="6">
         <v>0.315991970009668</v>
@@ -8194,8 +11536,26 @@
       <c r="J18">
         <v>0.43698312231026898</v>
       </c>
+      <c r="K18">
+        <v>0.31835093492334599</v>
+      </c>
+      <c r="L18">
+        <v>0.35170059208357202</v>
+      </c>
+      <c r="M18" s="6">
+        <v>0.276510779757418</v>
+      </c>
+      <c r="N18">
+        <v>0.313861873404435</v>
+      </c>
+      <c r="O18">
+        <v>0.352882072749854</v>
+      </c>
+      <c r="P18">
+        <v>0.38660963517340302</v>
+      </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -8209,10 +11569,10 @@
         <v>0.51829573934837103</v>
       </c>
       <c r="E19">
-        <v>0.14887218045112699</v>
-      </c>
-      <c r="F19">
-        <v>0.22456140350877099</v>
+        <v>0.13233082706766899</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0.22406015037593899</v>
       </c>
       <c r="G19">
         <v>-0.40100250626566403</v>
@@ -8226,8 +11586,26 @@
       <c r="J19">
         <v>-0.40100250626566403</v>
       </c>
+      <c r="K19" s="6">
+        <v>-0.39999999999999902</v>
+      </c>
+      <c r="L19">
+        <v>-0.42606516290726798</v>
+      </c>
+      <c r="M19" s="6">
+        <v>-0.39999999999999902</v>
+      </c>
+      <c r="N19">
+        <v>-0.40150375939849597</v>
+      </c>
+      <c r="O19">
+        <v>-0.40050125313283202</v>
+      </c>
+      <c r="P19">
+        <v>-0.40050125313283103</v>
+      </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -8241,10 +11619,10 @@
         <v>0.88339920948616502</v>
       </c>
       <c r="E20">
-        <v>0.55335968379446598</v>
+        <v>0.57114624505928901</v>
       </c>
       <c r="F20">
-        <v>0.48023715415019802</v>
+        <v>0.53557312252964395</v>
       </c>
       <c r="G20">
         <v>0.61264822134387398</v>
@@ -8258,8 +11636,26 @@
       <c r="J20">
         <v>0.55533596837944699</v>
       </c>
+      <c r="K20">
+        <v>3.5573122529644001E-2</v>
+      </c>
+      <c r="L20">
+        <v>0.16403162055336001</v>
+      </c>
+      <c r="M20">
+        <v>3.9525691699605001E-2</v>
+      </c>
+      <c r="N20">
+        <v>0.158102766798419</v>
+      </c>
+      <c r="O20" s="6">
+        <v>0.16798418972331999</v>
+      </c>
+      <c r="P20">
+        <v>0.122529644268775</v>
+      </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>31</v>
       </c>
@@ -8270,10 +11666,10 @@
         <v>0.72325375773651601</v>
       </c>
       <c r="E21">
-        <v>0.28404067197170602</v>
+        <v>0.29310344827586199</v>
       </c>
       <c r="F21">
-        <v>0.249115826702034</v>
+        <v>0.26105216622458</v>
       </c>
       <c r="G21">
         <v>0.365605658709107</v>
@@ -8287,8 +11683,26 @@
       <c r="J21">
         <v>0.33333333333333298</v>
       </c>
+      <c r="K21">
+        <v>1.10521662245799E-2</v>
+      </c>
+      <c r="L21">
+        <v>5.4155614500441998E-2</v>
+      </c>
+      <c r="M21">
+        <v>1.525198938992E-2</v>
+      </c>
+      <c r="N21">
+        <v>5.3050397877983997E-2</v>
+      </c>
+      <c r="O21">
+        <v>3.8682581786029999E-2</v>
+      </c>
+      <c r="P21">
+        <v>3.2272325375774E-2</v>
+      </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>32</v>
       </c>
@@ -8299,10 +11713,10 @@
         <v>0.46949602122015899</v>
       </c>
       <c r="E22">
-        <v>2.3872679045093E-2</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
+        <v>1.9893899204244E-2</v>
+      </c>
+      <c r="F22" s="6">
+        <v>2.6525198938989998E-3</v>
       </c>
       <c r="G22">
         <v>9.0185676392572994E-2</v>
@@ -8316,8 +11730,26 @@
       <c r="J22">
         <v>0.110079575596817</v>
       </c>
+      <c r="K22">
+        <v>1.4588859416446E-2</v>
+      </c>
+      <c r="L22" s="6">
+        <v>3.9787798408489998E-3</v>
+      </c>
+      <c r="M22" s="6">
+        <v>6.6312997347479996E-3</v>
+      </c>
+      <c r="N22" s="6">
+        <v>5.3050397877979997E-3</v>
+      </c>
+      <c r="O22" s="6">
+        <v>6.6312997347479996E-3</v>
+      </c>
+      <c r="P22" s="6">
+        <v>3.9787798408489998E-3</v>
+      </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>33</v>
       </c>
@@ -8328,10 +11760,10 @@
         <v>0.319148936170213</v>
       </c>
       <c r="E23">
-        <v>0.12720240653201501</v>
+        <v>0.120326600773528</v>
       </c>
       <c r="F23">
-        <v>0.16931671680275001</v>
+        <v>0.169746454662656</v>
       </c>
       <c r="G23">
         <v>0.175333046841427</v>
@@ -8344,6 +11776,24 @@
       </c>
       <c r="J23">
         <v>0.31070047271164603</v>
+      </c>
+      <c r="K23">
+        <v>3.9965620971208003E-2</v>
+      </c>
+      <c r="L23">
+        <v>5.4576708207992902E-2</v>
+      </c>
+      <c r="M23">
+        <v>4.254404813064E-2</v>
+      </c>
+      <c r="N23">
+        <v>6.5320154705630004E-2</v>
+      </c>
+      <c r="O23">
+        <v>7.2625698324022006E-2</v>
+      </c>
+      <c r="P23">
+        <v>5.5006446067898999E-2</v>
       </c>
     </row>
   </sheetData>
@@ -8357,7 +11807,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8372,7 +11822,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8387,7 +11837,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8402,7 +11852,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8417,7 +11867,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8431,8 +11881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EC3138-B95A-4C3F-B2E7-931683C074F7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>